<commit_message>
Update FORMATO 5B IES JOSE MARIA ARGUEDAS CHUQUIBAMBILLA - MAMARA.xlsx
</commit_message>
<xml_diff>
--- a/12.0 FORMATO N°05 REGISTRO AGREGADO DE IDEAS/FORMATO 5B IES JOSE MARIA ARGUEDAS CHUQUIBAMBILLA - MAMARA.xlsx
+++ b/12.0 FORMATO N°05 REGISTRO AGREGADO DE IDEAS/FORMATO 5B IES JOSE MARIA ARGUEDAS CHUQUIBAMBILLA - MAMARA.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'F05 IDEA IOARR'!$A$1:$M$104</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -565,7 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -662,9 +662,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,11 +725,38 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -743,101 +767,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1152,13 +1146,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A77" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="48" customWidth="1"/>
     <col min="2" max="4" width="22" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
@@ -1170,66 +1164,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="71"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="74"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="80"/>
     </row>
     <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="74"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="80"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
@@ -1255,17 +1249,17 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="84" t="s">
+      <c r="F7" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
@@ -1301,19 +1295,19 @@
       <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1335,17 +1329,17 @@
         <v>10</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="60"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1353,17 +1347,17 @@
         <v>11</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="60"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="68"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1371,17 +1365,17 @@
         <v>12</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="60"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="68"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1389,17 +1383,17 @@
         <v>13</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="60"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="68"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
@@ -1433,19 +1427,19 @@
       <c r="A18" s="4">
         <v>3</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
@@ -1463,21 +1457,21 @@
     </row>
     <row r="20" spans="1:12" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="91" t="s">
+      <c r="B20" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="63" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="65"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="89"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
@@ -1493,21 +1487,21 @@
     </row>
     <row r="22" spans="1:12" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
       <c r="G22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="66" t="s">
+      <c r="H22" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="68"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="87"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
@@ -1548,7 +1542,7 @@
       <c r="K24" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="L24" s="55">
+      <c r="L24" s="54">
         <v>1</v>
       </c>
     </row>
@@ -1574,7 +1568,7 @@
       <c r="G26" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H26" s="54">
+      <c r="H26" s="53">
         <v>0.2</v>
       </c>
       <c r="I26" s="24"/>
@@ -1614,19 +1608,19 @@
       <c r="A29" s="4">
         <v>4</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
@@ -1648,17 +1642,17 @@
         <v>4</v>
       </c>
       <c r="C31" s="28"/>
-      <c r="D31" s="58" t="s">
+      <c r="D31" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="60"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="68"/>
     </row>
     <row r="32" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
@@ -1666,17 +1660,17 @@
         <v>5</v>
       </c>
       <c r="C32" s="28"/>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="60"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="68"/>
     </row>
     <row r="33" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
@@ -1684,17 +1678,17 @@
         <v>6</v>
       </c>
       <c r="C33" s="28"/>
-      <c r="D33" s="58" t="s">
+      <c r="D33" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="60"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="68"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
@@ -1702,17 +1696,17 @@
         <v>7</v>
       </c>
       <c r="C34" s="28"/>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="60"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="68"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="27"/>
@@ -1746,19 +1740,19 @@
       <c r="A37" s="4">
         <v>5</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
@@ -1780,17 +1774,17 @@
         <v>4</v>
       </c>
       <c r="C39" s="28"/>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="60"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="68"/>
     </row>
     <row r="40" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="27"/>
@@ -1798,17 +1792,17 @@
         <v>5</v>
       </c>
       <c r="C40" s="28"/>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="59"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="60"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="68"/>
     </row>
     <row r="41" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
@@ -1816,17 +1810,17 @@
         <v>8</v>
       </c>
       <c r="C41" s="28"/>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="60"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="67"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="68"/>
     </row>
     <row r="42" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
@@ -1834,17 +1828,17 @@
         <v>9</v>
       </c>
       <c r="C42" s="28"/>
-      <c r="D42" s="58" t="s">
+      <c r="D42" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="60"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="68"/>
     </row>
     <row r="43" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
@@ -1878,19 +1872,19 @@
       <c r="A45" s="4">
         <v>6</v>
       </c>
-      <c r="B45" s="56" t="s">
+      <c r="B45" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
     </row>
     <row r="46" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
@@ -1912,17 +1906,17 @@
         <v>4</v>
       </c>
       <c r="C47" s="28"/>
-      <c r="D47" s="58" t="s">
+      <c r="D47" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="60"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="67"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="68"/>
     </row>
     <row r="48" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="27"/>
@@ -1930,17 +1924,17 @@
         <v>5</v>
       </c>
       <c r="C48" s="28"/>
-      <c r="D48" s="58" t="s">
+      <c r="D48" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="60"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="68"/>
     </row>
     <row r="49" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
@@ -1948,17 +1942,17 @@
         <v>3</v>
       </c>
       <c r="C49" s="28"/>
-      <c r="D49" s="58" t="s">
+      <c r="D49" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="59"/>
-      <c r="K49" s="59"/>
-      <c r="L49" s="60"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="68"/>
     </row>
     <row r="50" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
@@ -1992,19 +1986,19 @@
       <c r="A52" s="4">
         <v>7</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-      <c r="L52" s="56"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="62"/>
     </row>
     <row r="53" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
@@ -2028,13 +2022,13 @@
       <c r="C54" s="27"/>
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
-      <c r="H54" s="61"/>
-      <c r="I54" s="61"/>
-      <c r="J54" s="61"/>
-      <c r="K54" s="61"/>
-      <c r="L54" s="61"/>
+      <c r="F54" s="88"/>
+      <c r="G54" s="88"/>
+      <c r="H54" s="88"/>
+      <c r="I54" s="88"/>
+      <c r="J54" s="88"/>
+      <c r="K54" s="88"/>
+      <c r="L54" s="88"/>
     </row>
     <row r="55" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
@@ -2054,14 +2048,14 @@
     </row>
     <row r="56" spans="1:12" s="29" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11"/>
+      <c r="C56" s="90"/>
+      <c r="D56" s="90"/>
+      <c r="E56" s="90"/>
+      <c r="F56" s="90"/>
+      <c r="G56" s="90"/>
       <c r="H56" s="11"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
@@ -2100,13 +2094,13 @@
     </row>
     <row r="59" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="34" t="s">
         <v>47</v>
       </c>
       <c r="E59" s="27"/>
@@ -2120,13 +2114,13 @@
     </row>
     <row r="60" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="50" t="s">
+      <c r="C60" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="50" t="s">
+      <c r="D60" s="49" t="s">
         <v>89</v>
       </c>
       <c r="E60" s="27"/>
@@ -2169,19 +2163,19 @@
       <c r="A63" s="4">
         <v>8</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="56"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="56"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="62"/>
+      <c r="E63" s="62"/>
+      <c r="F63" s="62"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="62"/>
+      <c r="K63" s="62"/>
+      <c r="L63" s="62"/>
     </row>
     <row r="64" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
@@ -2196,85 +2190,85 @@
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:12" s="36" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" s="35" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
-      <c r="B65" s="80" t="s">
+      <c r="B65" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C65" s="80"/>
-      <c r="D65" s="80"/>
-      <c r="E65" s="84" t="s">
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="F65" s="85"/>
-      <c r="G65" s="78"/>
-      <c r="H65" s="78"/>
-      <c r="I65" s="78"/>
-      <c r="J65" s="78"/>
-      <c r="K65" s="78"/>
-      <c r="L65" s="78"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="65"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="65"/>
+      <c r="J65" s="65"/>
+      <c r="K65" s="65"/>
+      <c r="L65" s="65"/>
     </row>
     <row r="66" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="57" t="s">
+      <c r="B66" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="51">
+      <c r="C66" s="61"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="50">
         <v>380539.3</v>
       </c>
       <c r="F66" s="28"/>
-      <c r="G66" s="62">
+      <c r="G66" s="73">
         <v>699</v>
       </c>
-      <c r="H66" s="62"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="79"/>
-      <c r="K66" s="79"/>
-      <c r="L66" s="79"/>
+      <c r="H66" s="73"/>
+      <c r="I66" s="73"/>
+      <c r="J66" s="74"/>
+      <c r="K66" s="74"/>
+      <c r="L66" s="74"/>
     </row>
     <row r="67" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="57"/>
-      <c r="C67" s="57"/>
-      <c r="D67" s="57"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
       <c r="E67" s="33"/>
       <c r="F67" s="28"/>
-      <c r="G67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="79"/>
-      <c r="K67" s="79"/>
-      <c r="L67" s="79"/>
+      <c r="G67" s="73"/>
+      <c r="H67" s="73"/>
+      <c r="I67" s="73"/>
+      <c r="J67" s="74"/>
+      <c r="K67" s="74"/>
+      <c r="L67" s="74"/>
     </row>
     <row r="68" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="57"/>
-      <c r="C68" s="57"/>
-      <c r="D68" s="57"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="61"/>
+      <c r="D68" s="61"/>
       <c r="E68" s="33"/>
       <c r="F68" s="28"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="62"/>
-      <c r="J68" s="79"/>
-      <c r="K68" s="79"/>
-      <c r="L68" s="79"/>
+      <c r="G68" s="73"/>
+      <c r="H68" s="73"/>
+      <c r="I68" s="73"/>
+      <c r="J68" s="74"/>
+      <c r="K68" s="74"/>
+      <c r="L68" s="74"/>
     </row>
     <row r="69" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="57"/>
-      <c r="C69" s="57"/>
-      <c r="D69" s="57"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="61"/>
+      <c r="D69" s="61"/>
       <c r="E69" s="33"/>
       <c r="F69" s="28"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="62"/>
-      <c r="I69" s="62"/>
-      <c r="J69" s="79"/>
-      <c r="K69" s="79"/>
-      <c r="L69" s="79"/>
+      <c r="G69" s="73"/>
+      <c r="H69" s="73"/>
+      <c r="I69" s="73"/>
+      <c r="J69" s="74"/>
+      <c r="K69" s="74"/>
+      <c r="L69" s="74"/>
     </row>
     <row r="70" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
@@ -2293,23 +2287,23 @@
       <c r="A71" s="4">
         <v>9</v>
       </c>
-      <c r="B71" s="56" t="s">
+      <c r="B71" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="56"/>
-      <c r="I71" s="56"/>
-      <c r="J71" s="56"/>
-      <c r="K71" s="56"/>
-      <c r="L71" s="56"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="62"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="62"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="62"/>
+      <c r="K71" s="62"/>
+      <c r="L71" s="62"/>
     </row>
     <row r="72" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
-      <c r="B72" s="37"/>
+      <c r="B72" s="36"/>
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
@@ -2322,105 +2316,105 @@
     </row>
     <row r="73" spans="1:12" s="29" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
-      <c r="B73" s="80" t="s">
+      <c r="B73" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C73" s="80"/>
-      <c r="D73" s="80"/>
-      <c r="E73" s="84" t="s">
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="F73" s="85"/>
-      <c r="G73" s="90"/>
-      <c r="H73" s="78"/>
-      <c r="I73" s="78"/>
-      <c r="J73" s="78"/>
-      <c r="K73" s="78"/>
-      <c r="L73" s="78"/>
+      <c r="F73" s="60"/>
+      <c r="G73" s="64"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="65"/>
+      <c r="J73" s="65"/>
+      <c r="K73" s="65"/>
+      <c r="L73" s="65"/>
     </row>
     <row r="74" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
-      <c r="B74" s="57" t="s">
+      <c r="B74" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="84" t="s">
+      <c r="C74" s="61"/>
+      <c r="D74" s="61"/>
+      <c r="E74" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="F74" s="85"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="39"/>
-      <c r="K74" s="39"/>
-      <c r="L74" s="39"/>
+      <c r="F74" s="60"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
+      <c r="L74" s="38"/>
     </row>
     <row r="75" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
-      <c r="B75" s="57" t="s">
+      <c r="B75" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
       <c r="E75" s="33"/>
       <c r="F75" s="28"/>
-      <c r="G75" s="83">
+      <c r="G75" s="72">
         <v>699</v>
       </c>
-      <c r="H75" s="62"/>
-      <c r="I75" s="62"/>
-      <c r="J75" s="79"/>
-      <c r="K75" s="79"/>
-      <c r="L75" s="79"/>
+      <c r="H75" s="73"/>
+      <c r="I75" s="73"/>
+      <c r="J75" s="74"/>
+      <c r="K75" s="74"/>
+      <c r="L75" s="74"/>
     </row>
     <row r="76" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
-      <c r="B76" s="57" t="s">
+      <c r="B76" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C76" s="57"/>
-      <c r="D76" s="57"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="61"/>
       <c r="E76" s="33"/>
       <c r="F76" s="28"/>
-      <c r="G76" s="83"/>
-      <c r="H76" s="62"/>
-      <c r="I76" s="62"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="79"/>
-      <c r="L76" s="79"/>
+      <c r="G76" s="72"/>
+      <c r="H76" s="73"/>
+      <c r="I76" s="73"/>
+      <c r="J76" s="74"/>
+      <c r="K76" s="74"/>
+      <c r="L76" s="74"/>
     </row>
     <row r="77" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
-      <c r="B77" s="57" t="s">
+      <c r="B77" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C77" s="57"/>
-      <c r="D77" s="57"/>
+      <c r="C77" s="61"/>
+      <c r="D77" s="61"/>
       <c r="E77" s="33"/>
       <c r="F77" s="28"/>
-      <c r="G77" s="83"/>
-      <c r="H77" s="62"/>
-      <c r="I77" s="62"/>
-      <c r="J77" s="79"/>
-      <c r="K77" s="79"/>
-      <c r="L77" s="79"/>
+      <c r="G77" s="72"/>
+      <c r="H77" s="73"/>
+      <c r="I77" s="73"/>
+      <c r="J77" s="74"/>
+      <c r="K77" s="74"/>
+      <c r="L77" s="74"/>
     </row>
     <row r="78" spans="1:12" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
-      <c r="B78" s="57" t="s">
+      <c r="B78" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="C78" s="57"/>
-      <c r="D78" s="57"/>
+      <c r="C78" s="61"/>
+      <c r="D78" s="61"/>
       <c r="E78" s="33"/>
       <c r="F78" s="28"/>
-      <c r="G78" s="83"/>
-      <c r="H78" s="62"/>
-      <c r="I78" s="62"/>
-      <c r="J78" s="79"/>
-      <c r="K78" s="79"/>
-      <c r="L78" s="79"/>
+      <c r="G78" s="72"/>
+      <c r="H78" s="73"/>
+      <c r="I78" s="73"/>
+      <c r="J78" s="74"/>
+      <c r="K78" s="74"/>
+      <c r="L78" s="74"/>
     </row>
     <row r="79" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
@@ -2452,7 +2446,7 @@
       <c r="A81" s="4">
         <v>10</v>
       </c>
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="39" t="s">
         <v>32</v>
       </c>
       <c r="C81" s="31"/>
@@ -2480,15 +2474,15 @@
     </row>
     <row r="83" spans="1:14" s="29" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
-      <c r="B83" s="86" t="s">
+      <c r="B83" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C83" s="87"/>
-      <c r="D83" s="88"/>
-      <c r="E83" s="84" t="s">
+      <c r="C83" s="56"/>
+      <c r="D83" s="57"/>
+      <c r="E83" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="F83" s="85"/>
+      <c r="F83" s="60"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
       <c r="J83" s="6"/>
@@ -2497,15 +2491,15 @@
     </row>
     <row r="84" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
-      <c r="B84" s="41" t="s">
+      <c r="B84" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C84" s="42"/>
-      <c r="D84" s="42"/>
-      <c r="E84" s="84" t="s">
+      <c r="C84" s="41"/>
+      <c r="D84" s="41"/>
+      <c r="E84" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="F84" s="85"/>
+      <c r="F84" s="60"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
       <c r="J84" s="6"/>
@@ -2517,8 +2511,8 @@
       <c r="B85" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
       <c r="E85" s="33"/>
       <c r="F85" s="28"/>
       <c r="G85" s="12"/>
@@ -2529,7 +2523,7 @@
     </row>
     <row r="86" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
-      <c r="B86" s="44" t="s">
+      <c r="B86" s="43" t="s">
         <v>38</v>
       </c>
       <c r="C86" s="12"/>
@@ -2547,8 +2541,8 @@
       <c r="B87" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
       <c r="E87" s="33"/>
       <c r="F87" s="28"/>
       <c r="G87" s="12"/>
@@ -2559,11 +2553,11 @@
     </row>
     <row r="88" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
-      <c r="B88" s="45" t="s">
+      <c r="B88" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C88" s="46"/>
-      <c r="D88" s="46"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="45"/>
       <c r="E88" s="33"/>
       <c r="F88" s="28"/>
       <c r="G88" s="12"/>
@@ -2589,21 +2583,21 @@
       <c r="A90" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B90" s="56" t="s">
+      <c r="B90" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="56"/>
-      <c r="F90" s="56"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="56"/>
-      <c r="I90" s="56"/>
-      <c r="J90" s="56"/>
-      <c r="K90" s="56"/>
-      <c r="L90" s="56"/>
-      <c r="M90" s="56"/>
-      <c r="N90" s="56"/>
+      <c r="C90" s="62"/>
+      <c r="D90" s="62"/>
+      <c r="E90" s="62"/>
+      <c r="F90" s="62"/>
+      <c r="G90" s="62"/>
+      <c r="H90" s="62"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="62"/>
+      <c r="K90" s="62"/>
+      <c r="L90" s="62"/>
+      <c r="M90" s="62"/>
+      <c r="N90" s="62"/>
     </row>
     <row r="91" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
@@ -2623,32 +2617,32 @@
       <c r="B92" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C92" s="47"/>
+      <c r="C92" s="46"/>
       <c r="D92" s="31"/>
-      <c r="E92" s="75" t="s">
+      <c r="E92" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="F92" s="75"/>
-      <c r="G92" s="75"/>
-      <c r="H92" s="75"/>
-      <c r="I92" s="75"/>
-      <c r="J92" s="75"/>
-      <c r="K92" s="75"/>
-      <c r="L92" s="75"/>
+      <c r="F92" s="81"/>
+      <c r="G92" s="81"/>
+      <c r="H92" s="81"/>
+      <c r="I92" s="81"/>
+      <c r="J92" s="81"/>
+      <c r="K92" s="81"/>
+      <c r="L92" s="81"/>
     </row>
     <row r="93" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="25"/>
       <c r="C93" s="31"/>
       <c r="D93" s="31"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="75"/>
-      <c r="G93" s="75"/>
-      <c r="H93" s="75"/>
-      <c r="I93" s="75"/>
-      <c r="J93" s="75"/>
-      <c r="K93" s="75"/>
-      <c r="L93" s="75"/>
+      <c r="E93" s="81"/>
+      <c r="F93" s="81"/>
+      <c r="G93" s="81"/>
+      <c r="H93" s="81"/>
+      <c r="I93" s="81"/>
+      <c r="J93" s="81"/>
+      <c r="K93" s="81"/>
+      <c r="L93" s="81"/>
     </row>
     <row r="94" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
@@ -2668,7 +2662,7 @@
       <c r="B95" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C95" s="52" t="s">
+      <c r="C95" s="51" t="s">
         <v>80</v>
       </c>
       <c r="D95" s="31"/>
@@ -2697,26 +2691,26 @@
       <c r="L96" s="6"/>
     </row>
     <row r="97" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="48" t="s">
+      <c r="A97" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B97" s="82" t="s">
+      <c r="B97" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C97" s="82"/>
-      <c r="D97" s="82"/>
-      <c r="E97" s="82"/>
-      <c r="F97" s="82"/>
-      <c r="G97" s="82"/>
-      <c r="H97" s="82"/>
-      <c r="I97" s="82"/>
-      <c r="J97" s="82"/>
-      <c r="K97" s="82"/>
-      <c r="L97" s="82"/>
-      <c r="M97" s="82"/>
-      <c r="N97" s="82"/>
-      <c r="O97" s="82"/>
-      <c r="P97" s="82"/>
+      <c r="C97" s="71"/>
+      <c r="D97" s="71"/>
+      <c r="E97" s="71"/>
+      <c r="F97" s="71"/>
+      <c r="G97" s="71"/>
+      <c r="H97" s="71"/>
+      <c r="I97" s="71"/>
+      <c r="J97" s="71"/>
+      <c r="K97" s="71"/>
+      <c r="L97" s="71"/>
+      <c r="M97" s="71"/>
+      <c r="N97" s="71"/>
+      <c r="O97" s="71"/>
+      <c r="P97" s="71"/>
     </row>
     <row r="98" spans="1:16" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="27"/>
@@ -2791,7 +2785,64 @@
       <c r="I103" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="73">
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="D15:L15"/>
+    <mergeCell ref="F54:L54"/>
+    <mergeCell ref="B52:L52"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="D40:L40"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B63:L63"/>
+    <mergeCell ref="D48:L48"/>
+    <mergeCell ref="D49:L49"/>
+    <mergeCell ref="G20:L20"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="D31:L31"/>
+    <mergeCell ref="D32:L32"/>
+    <mergeCell ref="D33:L33"/>
+    <mergeCell ref="D34:L34"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L4"/>
+    <mergeCell ref="E92:L93"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="J66:L66"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="J68:L68"/>
+    <mergeCell ref="J69:L69"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="D41:L41"/>
+    <mergeCell ref="D42:L42"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B97:P97"/>
+    <mergeCell ref="B90:N90"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="G76:I76"/>
+    <mergeCell ref="J76:L76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="G77:I77"/>
+    <mergeCell ref="J77:L77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="G78:I78"/>
+    <mergeCell ref="J78:L78"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E83:F83"/>
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="F7:L7"/>
     <mergeCell ref="B74:D74"/>
@@ -2808,67 +2859,11 @@
     <mergeCell ref="B67:D67"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="D47:L47"/>
-    <mergeCell ref="B97:P97"/>
-    <mergeCell ref="B90:N90"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="G75:I75"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="G76:I76"/>
-    <mergeCell ref="J76:L76"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="G77:I77"/>
-    <mergeCell ref="J77:L77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="G78:I78"/>
-    <mergeCell ref="J78:L78"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L4"/>
-    <mergeCell ref="E92:L93"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="J66:L66"/>
-    <mergeCell ref="J67:L67"/>
-    <mergeCell ref="J68:L68"/>
-    <mergeCell ref="J69:L69"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="D41:L41"/>
-    <mergeCell ref="D42:L42"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="D48:L48"/>
-    <mergeCell ref="D49:L49"/>
-    <mergeCell ref="G20:L20"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="D31:L31"/>
-    <mergeCell ref="D32:L32"/>
-    <mergeCell ref="D33:L33"/>
-    <mergeCell ref="D34:L34"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="D15:L15"/>
-    <mergeCell ref="F54:L54"/>
-    <mergeCell ref="B52:L52"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="D40:L40"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B63:L63"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
     <brk id="36" max="12" man="1"/>

</xml_diff>